<commit_message>
updated parsing script; proceeded with coding
</commit_message>
<xml_diff>
--- a/data/tagging_system.xlsx
+++ b/data/tagging_system.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\2022_Fall\65411\data\data_in_use\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\2022_Fall\65411\QSSS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DEC2CE-B2AD-45AC-A50F-0DCE381D9F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1A73F-B3C4-437C-9F40-EAAE1E575A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24" yWindow="0" windowWidth="9048" windowHeight="11004" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tags" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,10 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FutureWork</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Intro</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,124 +83,260 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>MethDef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Justification of methods and/or models used</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResInf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Suggestions on future work directions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Struct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structural signals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hard to classify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Section</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Course</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36-200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discussion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research Scenarios</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataDesc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MethJust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FuWork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As the world continues to transform into a generation of digitally-centered people, social platforms are beginning to grasp the time and attention of many: YouTube being a popular choice.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>With the growing effects of climate change, natural disasters will increase in frequency and severity in the coming years.</t>
+  </si>
+  <si>
+    <t>As the global population increases, the need to identify and categorize areas where deadly wildfires are likely to occur is critical to ensuring their damage to life and property is mitigated.</t>
+  </si>
+  <si>
+    <t>This work may be helpful to creators looking to join the ever-growing world of YouTube.</t>
+  </si>
+  <si>
+    <t>Our goal therefore from this report is to better understand the behavior and impact of the number of subscribers.</t>
+  </si>
+  <si>
+    <t>The first question of this report considers the distribution of the “area” variable.</t>
+  </si>
+  <si>
+    <t>HypDef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HypJust</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>We hypothesized that as we age, we suffer more health issues that can lead to more hospital stays.</t>
+  </si>
+  <si>
+    <t>Reasoning behind the proposed hypothesis</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Since YouTube contains a variety of content and people are making use of the platform for many different purposes, we can expect videos in different channel categories to bring different audience sizes.</t>
+  </si>
+  <si>
+    <t>We have the information on 788 health insurance subscribers from the period of Janurary 1998 to December 1999.</t>
+  </si>
+  <si>
+    <t>Description of dataset(s) and variable(s) used</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age is a quantitative variable that measuring the age of subscribers.</t>
+  </si>
+  <si>
+    <t>This is because conditions during summer appear to be more conducive to wildfires — hotter and drier days — and vice versa for winter.</t>
+  </si>
+  <si>
+    <t>The relationship between two quantitative variables could be represented by a scatterplot.</t>
+  </si>
+  <si>
+    <t>We used a scatterplot to compare the relationship between Age and Duration of Stay.</t>
+  </si>
+  <si>
+    <t>However, as we measure severity, not frequency, we need to analyze the area variable, as what matters is not the number of fires but how many hectares are burnt.</t>
+  </si>
+  <si>
+    <t>The mean number of subscribers was 3201757 subscribers, and the standard deviation of the subscribers was 3556605 subscribers.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>However, after calculating correlation, we find that there is only a -0.076 linear correlation between RH and area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After performing our test, we are given an F-Score of 1.9021 which is relatively large for this situation and a p-value of 0.0026. </t>
+  </si>
+  <si>
+    <t>Based on the chi-square test, with a chi-squared value of 36.109 and a p-value of 0.00000009034, we can reject the null hypothesis that there is no association between these variables;</t>
+  </si>
+  <si>
+    <t>Montesinho National Park is not representative of all global forests or even of all forests in Portugal.</t>
+  </si>
+  <si>
+    <t>The relationship concluded as a result of this data, however, was limiting in the sense that other factors that would largely affect viewsPerVideo were not accounted for.</t>
+  </si>
+  <si>
+    <t>Concerning the small peak in March, a possible explanation this report suggests is that there may be several weeks in March where there is a sudden heatwave or other cyclic condition that lends itself to greater severity fires.</t>
+  </si>
+  <si>
+    <t>As the plot isn’t linear, we cannot conclude that there is a relationship between age and duration.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>This work can be further built on using new data using newer analysis models or using the same models by building hypotheses in the given data.</t>
+  </si>
+  <si>
+    <t>For this study, we would have appreciated data being collected from more sources (to avoid bias from one sample station), data from several forests around the globe, and for data to have been collected from a longer period of time.</t>
+  </si>
+  <si>
+    <t>Presentation of descriptive results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presentation of statistical inference results</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statement of research hypothesis; does not need to mention statistical significance; does not need to be directional</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 1, located above, displays the mean and standard deviation in viewsPerVideo of each channel category, and there are a few notable features.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>This [standard deviation] is on average how far the data tends to stray away from the mean.</t>
+  </si>
+  <si>
     <t>Definition of methods and/or models used</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MethDef</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MethJust</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Justification of methods and/or models used</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presentation of descriptive results</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResInf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResDesc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presentation of statistical inference results</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretation of results or general conclusion in context</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reflections on limitations of the current work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Suggestions on future work directions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Struct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Structural signals</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hard to classify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Section</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Course</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>36-200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discussion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Research Scenarios</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResDesc(Viz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResInf(Viz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presentation of descriptive results (with graphs)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presentation of statistical inference results (with graphs)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DataDesc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description of dataset(s) used</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RQNat</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rationale behind the proposed research question</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>5-fold cross validation will also be used to determine which of the models fit best to the data, in terms of prediction error.</t>
+  </si>
+  <si>
+    <t>(36-200 only) The second question of this report considers whether the month of the year is associated with fire severity and, if so, identifies their relationship.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LimData</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LimAna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflections on limitations of the dataset available</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflections on limitations of the current analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntVar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntImp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretation of results, only in terms of immediate context, e.g., in terms of the meanings of the variables</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretation of results, in terms of general conclusion or implication</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataStat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistical description of variables, usually through univariate EDA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The mean duration is 164 days and the standard deviation of duration is 120.916 days.</t>
+  </si>
+  <si>
+    <t>This confirms how only a few amount of channels are successfully able to maintain a high engagement, or a large view per video count.</t>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Section titles (used for discarding titles after coding and before training)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Following this summarization of the dataset, we discuss the formal hypothesis now.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The data analysis could have been improved by going more into depth within each continent or even country- for example, observing the user base of individual states within the United States</t>
+  </si>
+  <si>
+    <t>Note: All of the graphs in this section are zoomed in to show the relationships in the scatterplots better, since there are a large number of high outliers for the quantitative measures of success variables</t>
+  </si>
+  <si>
+    <t>The mean area value is 12.895 hectares, while the high range (1090.740) and far right-skewed data and high standard deviation (63.646) suggest that there are significant variations in-between fires</t>
   </si>
 </sst>
 </file>
@@ -231,6 +363,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,14 +395,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -282,15 +444,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}" name="表2" displayName="表2" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}" name="表2" displayName="表2" ref="A1:D19" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D19" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B2FA874C-ECFA-45F4-B2F3-3990C8816D4E}" name="Tag"/>
-    <tableColumn id="2" xr3:uid="{99B403F3-3559-4A90-BDF1-30951BCFD50A}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{6C5FC48A-4FB1-4ADD-9132-A67EC41AFB05}" name="Example1"/>
-    <tableColumn id="4" xr3:uid="{E50A41DB-197B-46F9-8D52-4FB53CB55762}" name="Example2"/>
+    <tableColumn id="1" xr3:uid="{B2FA874C-ECFA-45F4-B2F3-3990C8816D4E}" name="Tag" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{99B403F3-3559-4A90-BDF1-30951BCFD50A}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6C5FC48A-4FB1-4ADD-9132-A67EC41AFB05}" name="Example1" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E50A41DB-197B-46F9-8D52-4FB53CB55762}" name="Example2" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -568,18 +730,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="3" max="4" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -596,133 +757,263 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="55.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="55.2">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27.6">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="41.4">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="55.2">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41.4">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="55.2">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="41.4">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="41.4">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="41.4">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="55.2">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="41.4">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="69">
+      <c r="A14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="55.2">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="55.2">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="69">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="C17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="41.4">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="55.2">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="27.6">
+      <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -750,42 +1041,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned parser, requirements, and README
</commit_message>
<xml_diff>
--- a/data/tagging_system.xlsx
+++ b/data/tagging_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\2022_Fall\65411\QSSS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1A73F-B3C4-437C-9F40-EAAE1E575A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5283D69-05D8-4388-B319-5E591C7D98A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="0" windowWidth="9048" windowHeight="11004" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11064" yWindow="24" windowWidth="11976" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tags" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
   <si>
     <t>Tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,6 +337,46 @@
   </si>
   <si>
     <t>The mean area value is 12.895 hectares, while the high range (1090.740) and far right-skewed data and high standard deviation (63.646) suggest that there are significant variations in-between fires</t>
+  </si>
+  <si>
+    <t>Collapsed Tag</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lim</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Struct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Res</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RQDef</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RQJust</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -414,7 +454,10 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -444,10 +487,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}" name="表2" displayName="表2" ref="A1:D19" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D19" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B2FA874C-ECFA-45F4-B2F3-3990C8816D4E}" name="Tag" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}" name="表2" displayName="表2" ref="A1:E20" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E20" xr:uid="{58E5A221-C741-43D4-A1F2-7F6C12DB9932}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B2FA874C-ECFA-45F4-B2F3-3990C8816D4E}" name="Tag" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{BD0A62F0-DF7B-4E79-98AC-628B735A567C}" name="Collapsed Tag" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{99B403F3-3559-4A90-BDF1-30951BCFD50A}" name="Description" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{6C5FC48A-4FB1-4ADD-9132-A67EC41AFB05}" name="Example1" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{E50A41DB-197B-46F9-8D52-4FB53CB55762}" name="Example2" dataDxfId="0"/>
@@ -730,290 +774,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" customWidth="1"/>
-    <col min="3" max="4" width="50.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="55.2">
+    <row r="2" spans="1:5" ht="55.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="55.2">
+    <row r="3" spans="1:5" ht="55.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.6">
+    <row r="4" spans="1:5" ht="41.4">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="41.4">
+    <row r="5" spans="1:5" ht="55.2">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="55.2">
+    <row r="6" spans="1:5" ht="55.2">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="41.4">
+    <row r="7" spans="1:5" ht="41.4">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="55.2">
+    <row r="8" spans="1:5" ht="55.2">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="41.4">
+    <row r="9" spans="1:5" ht="41.4">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="41.4">
+    <row r="10" spans="1:5" ht="55.2">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="41.4">
+    <row r="11" spans="1:5" ht="41.4">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="55.2">
+    <row r="12" spans="1:5" ht="55.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="41.4">
+    <row r="13" spans="1:5" ht="55.2">
       <c r="A13" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="69">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="69">
       <c r="A14" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="55.2">
+    <row r="15" spans="1:5" ht="55.2">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="55.2">
+    <row r="16" spans="1:5" ht="55.2">
       <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="69">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="69">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="41.4">
+    <row r="18" spans="1:5" ht="41.4">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="55.2">
+    <row r="19" spans="1:5" ht="69">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="27.6">
+    <row r="20" spans="1:5" ht="41.4">
       <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>